<commit_message>
9.14.0-b5: Initial support for Pingon 14C ecxavator and more
</commit_message>
<xml_diff>
--- a/documentation/servoCurves.xlsx
+++ b/documentation/servoCurves.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5CF5E1-CED6-BA44-BC19-152540BCDAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91ED0EE8-1419-004E-8CD8-12E9D1A5F4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17020" yWindow="6780" windowWidth="28240" windowHeight="17240" activeTab="2" xr2:uid="{AFF9BAC0-96AD-154F-A6C1-184206A815AB}"/>
+    <workbookView xWindow="15720" yWindow="6520" windowWidth="32960" windowHeight="17240" activeTab="3" xr2:uid="{AFF9BAC0-96AD-154F-A6C1-184206A815AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Exponential Throttle" sheetId="2" r:id="rId1"/>
     <sheet name="Hydraulic Valve" sheetId="1" r:id="rId2"/>
     <sheet name="Hydraulic Valve (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="Hydraulic Pump" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>Servo curves</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Pump Mixer</t>
   </si>
 </sst>
 </file>
@@ -556,14 +563,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hydraulic Valve'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Input</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -572,62 +590,133 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>'Hydraulic Valve'!$B$5:$B$15</c:f>
+              <c:f>'Hydraulic Valve'!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>1100</c:v>
+                  <c:v>-50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1200</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1300</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1400</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1500</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1700</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1800</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1900</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000</c:v>
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hydraulic Valve'!$B$4:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8ED0-C347-88AD-A828C963912E}"/>
+              <c16:uniqueId val="{00000000-BD17-104B-A5DE-39FA4F142747}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hydraulic Valve'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>output</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -636,54 +725,114 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>'Hydraulic Valve'!$C$5:$C$15</c:f>
+              <c:f>'Hydraulic Valve'!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>1050</c:v>
+                  <c:v>-50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1100</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1150</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1200</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1500</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1850</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1900</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1950</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000</c:v>
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hydraulic Valve'!$C$4:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8ED0-C347-88AD-A828C963912E}"/>
+              <c16:uniqueId val="{00000001-BD17-104B-A5DE-39FA4F142747}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -695,17 +844,31 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1452484847"/>
-        <c:axId val="1453211551"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1452484847"/>
+        <c:axId val="358905728"/>
+        <c:axId val="358924384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="358905728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -714,8 +877,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -742,19 +905,16 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1453211551"/>
+        <c:crossAx val="358924384"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1453211551"/>
+        <c:axId val="358924384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2200"/>
-          <c:min val="800"/>
+          <c:max val="2000"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -778,8 +938,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -803,9 +969,9 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1452484847"/>
+        <c:crossAx val="358905728"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -937,14 +1103,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hydraulic Valve (2)'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Input</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -953,62 +1130,133 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>'Hydraulic Valve (2)'!$B$5:$B$15</c:f>
+              <c:f>'Hydraulic Valve (2)'!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>1100</c:v>
+                  <c:v>-50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1200</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1300</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1400</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1500</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1700</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1800</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1900</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000</c:v>
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hydraulic Valve (2)'!$B$4:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5E2B-724A-914F-20D08E5B4CC9}"/>
+              <c16:uniqueId val="{00000000-C0AB-2D41-90A1-DD32E35477C2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hydraulic Valve (2)'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>output</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1017,54 +1265,114 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>'Hydraulic Valve (2)'!$C$5:$C$15</c:f>
+              <c:f>'Hydraulic Valve (2)'!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>1025</c:v>
+                  <c:v>-50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1050</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1075</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1100</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1500</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1925</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1950</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1975</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000</c:v>
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hydraulic Valve (2)'!$C$4:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1925</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5E2B-724A-914F-20D08E5B4CC9}"/>
+              <c16:uniqueId val="{00000001-C0AB-2D41-90A1-DD32E35477C2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1076,17 +1384,31 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1452484847"/>
-        <c:axId val="1453211551"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1452484847"/>
+        <c:axId val="555975344"/>
+        <c:axId val="555977056"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="555975344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1095,8 +1417,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1123,19 +1445,16 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1453211551"/>
+        <c:crossAx val="555977056"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1453211551"/>
+        <c:axId val="555977056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2200"/>
-          <c:min val="800"/>
+          <c:max val="2000"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1159,8 +1478,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1184,9 +1509,477 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1452484847"/>
+        <c:crossAx val="555975344"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hydraulic Pump'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Input</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hydraulic Pump'!$A$4:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hydraulic Pump'!$B$4:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1550</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6DDC-D44B-9D1A-8C97C02B082C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hydraulic Pump'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Output</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hydraulic Pump'!$A$4:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hydraulic Pump'!$C$4:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6DDC-D44B-9D1A-8C97C02B082C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="358834480"/>
+        <c:axId val="358836192"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="358834480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358836192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="358836192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2000"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358834480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1391,6 +2184,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1908,7 +2741,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1935,8 +2768,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2016,11 +2849,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2031,11 +2859,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2047,7 +2870,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2067,9 +2890,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2082,10 +2902,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2125,22 +2945,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2245,8 +3066,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2378,19 +3199,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2404,6 +3226,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2424,7 +3257,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2451,8 +3284,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2532,11 +3365,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2547,11 +3375,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2563,7 +3386,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2583,9 +3406,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2598,10 +3418,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2641,22 +3461,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2761,8 +3582,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2894,19 +3715,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2920,6 +3742,533 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2986,23 +4335,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>543560</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>132080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
+      <xdr:rowOff>132080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>284480</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>132080</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>589280</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1">
+        <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4514C1A5-9C1A-E586-5258-37FC234948B9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D720FF5-6D6D-71CC-B854-4D13E3503288}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3027,29 +4376,68 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>543560</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>187960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>284480</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>132080</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>772160</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1">
+        <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C00B2BA-C524-804A-9862-527EBEC35161}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66DAF6C0-4D96-A50D-EB3E-451D23B0F1E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>197205</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>203484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>66828</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>188244</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72013918-03AD-5188-6D97-F7AEA70628C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3516,10 +4904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A011C2-F712-E94D-81B2-F55AFCD5B5F5}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3527,12 +4915,12 @@
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3542,8 +4930,11 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>0</v>
       </c>
@@ -3551,10 +4942,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f>(B5-1000)/10</f>
-        <v>0</v>
+        <f t="shared" ref="A5:A9" si="0">(B5-1500)/10</f>
+        <v>-50</v>
       </c>
       <c r="B5" s="1">
         <v>1000</v>
@@ -3562,11 +4953,15 @@
       <c r="C5" s="1">
         <v>1000</v>
       </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D9" si="1">(C5-1500)/10</f>
+        <v>-50</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f t="shared" ref="A6:A9" si="0">(B6-1000)/10</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>-40</v>
       </c>
       <c r="B6" s="1">
         <v>1100</v>
@@ -3574,11 +4969,15 @@
       <c r="C6" s="1">
         <v>1050</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>-45</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>-30</v>
       </c>
       <c r="B7" s="1">
         <v>1200</v>
@@ -3586,11 +4985,15 @@
       <c r="C7" s="1">
         <v>1100</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>-40</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>-20</v>
       </c>
       <c r="B8" s="1">
         <v>1300</v>
@@ -3598,11 +5001,15 @@
       <c r="C8" s="1">
         <v>1150</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>-35</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>-10</v>
       </c>
       <c r="B9" s="1">
         <v>1400</v>
@@ -3610,8 +5017,12 @@
       <c r="C9" s="1">
         <v>1200</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>-30</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>(B10-1500)/10</f>
         <v>0</v>
@@ -3622,10 +5033,14 @@
       <c r="C10" s="1">
         <v>1500</v>
       </c>
+      <c r="D10">
+        <f>(C10-1500)/10</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f t="shared" ref="A11:A15" si="1">(B11-1500)/10</f>
+        <f t="shared" ref="A11:A15" si="2">(B11-1500)/10</f>
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -3634,10 +5049,14 @@
       <c r="C11" s="1">
         <v>1800</v>
       </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D15" si="3">(C11-1500)/10</f>
+        <v>30</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="B12" s="1">
@@ -3646,10 +5065,14 @@
       <c r="C12" s="1">
         <v>1850</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B13" s="1">
@@ -3658,10 +5081,14 @@
       <c r="C13" s="1">
         <v>1900</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="B14" s="1">
@@ -3670,10 +5097,14 @@
       <c r="C14" s="1">
         <v>1950</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="B15" s="1">
@@ -3682,8 +5113,12 @@
       <c r="C15" s="1">
         <v>2000</v>
       </c>
+      <c r="D15">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>3000</v>
       </c>
@@ -3699,23 +5134,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5413717-D469-8640-9693-B6C42CEC1D4E}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3725,8 +5161,11 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>0</v>
       </c>
@@ -3734,10 +5173,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f>(B5-1000)/10</f>
-        <v>0</v>
+        <f t="shared" ref="A5:A9" si="0">(B5-1500)/10</f>
+        <v>-50</v>
       </c>
       <c r="B5" s="1">
         <v>1000</v>
@@ -3745,11 +5184,15 @@
       <c r="C5" s="1">
         <v>1000</v>
       </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D9" si="1">(C5-1500)/10</f>
+        <v>-50</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f t="shared" ref="A6:A9" si="0">(B6-1000)/10</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>-40</v>
       </c>
       <c r="B6" s="1">
         <v>1100</v>
@@ -3757,11 +5200,15 @@
       <c r="C6" s="1">
         <v>1025</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>-47.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>-30</v>
       </c>
       <c r="B7" s="1">
         <v>1200</v>
@@ -3769,11 +5216,15 @@
       <c r="C7" s="1">
         <v>1050</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>-45</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>-20</v>
       </c>
       <c r="B8" s="1">
         <v>1300</v>
@@ -3781,11 +5232,15 @@
       <c r="C8" s="1">
         <v>1075</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>-42.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>-10</v>
       </c>
       <c r="B9" s="1">
         <v>1400</v>
@@ -3793,8 +5248,12 @@
       <c r="C9" s="1">
         <v>1100</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>-40</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>(B10-1500)/10</f>
         <v>0</v>
@@ -3805,10 +5264,14 @@
       <c r="C10" s="1">
         <v>1500</v>
       </c>
+      <c r="D10">
+        <f>(C10-1500)/10</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f t="shared" ref="A11:A15" si="1">(B11-1500)/10</f>
+        <f t="shared" ref="A11:A15" si="2">(B11-1500)/10</f>
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -3817,10 +5280,14 @@
       <c r="C11" s="1">
         <v>1900</v>
       </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D15" si="3">(C11-1500)/10</f>
+        <v>40</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="B12" s="1">
@@ -3829,10 +5296,14 @@
       <c r="C12" s="1">
         <v>1925</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="3"/>
+        <v>42.5</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B13" s="1">
@@ -3841,10 +5312,14 @@
       <c r="C13" s="1">
         <v>1950</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="B14" s="1">
@@ -3853,25 +5328,168 @@
       <c r="C14" s="1">
         <v>1975</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="3"/>
+        <v>47.5</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909FD757-2ADD-474F-BBDB-679791CAAE80}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>(B5-1500)/10</f>
+        <v>-50</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D6" si="0">(C5-1500)/10</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" ref="A6:A9" si="1">(B6-1500)/10</f>
+        <v>-5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1450</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>(B7-1500)/10</f>
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D7">
+        <f>(C7-1500)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1550</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D9" si="2">(C8-1500)/10</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B9" s="1">
         <v>2000</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C9" s="1">
         <v>2000</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
         <v>3000</v>
       </c>
-      <c r="C16" s="1">
-        <v>3000</v>
+      <c r="C10" s="1">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>